<commit_message>
update: Add feature correlation
</commit_message>
<xml_diff>
--- a/analysis/result.xlsx
+++ b/analysis/result.xlsx
@@ -4,13 +4,12 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="COR Matrix" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Cor Result" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Day Trade" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="ITC Trade" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Day Trade" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="ITC Trade" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
   <si>
     <t>開盤價</t>
   </si>
@@ -96,24 +95,6 @@
   </si>
   <si>
     <t>投信買賣超</t>
-  </si>
-  <si>
-    <t>DayTrade&amp;漲幅 cor</t>
-  </si>
-  <si>
-    <t>投信庫存&amp;收盤價 cor</t>
-  </si>
-  <si>
-    <t>投信庫存&amp;最高價 cor</t>
-  </si>
-  <si>
-    <t>投信買賣超&amp;成交量 cor</t>
-  </si>
-  <si>
-    <t>投信買賣超&amp;收盤價 cor</t>
-  </si>
-  <si>
-    <t>投信買賣超&amp;漲幅 (whole)</t>
   </si>
   <si>
     <t>bank</t>
@@ -2851,7 +2832,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2859,91 +2840,342 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="s"/>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
       <c r="C2" t="n">
-        <v>-0.3547053916083732</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-0.3568291427348868</v>
-      </c>
-      <c r="E2" t="n">
-        <v>-0.01312009294491486</v>
-      </c>
-      <c r="F2" t="n">
-        <v>-0.01854965153713543</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.3099272502729289</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>-0.1192638217567127</v>
+      <c r="B3" t="s">
+        <v>29</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.3467047627208574</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-0.3482743123171997</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.07162144581193065</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.01223099193449412</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.3099272502729289</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B4" t="n">
-        <v>-0.07855237514798381</v>
-      </c>
-      <c r="C4" t="n">
-        <v>-0.3212108661659831</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-0.3251041036380728</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.005664378365373683</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.03761982553172273</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.3099272502729289</v>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" t="n">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2967,10 +3199,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2978,10 +3210,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C2" t="n">
-        <v>71</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2989,10 +3221,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C3" t="n">
-        <v>57</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3000,10 +3232,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C4" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3011,10 +3243,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C5" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3022,10 +3254,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C6" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3033,10 +3265,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C7" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3044,10 +3276,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C8" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3055,10 +3287,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C9" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3066,10 +3298,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C10" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -3077,10 +3309,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C11" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -3088,10 +3320,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C12" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -3099,10 +3331,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C13" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -3110,10 +3342,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="C14" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -3121,10 +3353,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C15" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -3132,10 +3364,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C16" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -3143,10 +3375,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C17" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -3154,10 +3386,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C18" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -3165,10 +3397,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -3176,10 +3408,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C20" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -3187,10 +3419,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C21" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -3198,10 +3430,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C22" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -3209,10 +3441,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C23" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -3220,7 +3452,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C24" t="n">
         <v>14</v>
@@ -3231,10 +3463,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C25" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -3242,10 +3474,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C26" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -3253,10 +3485,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C27" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -3264,10 +3496,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C28" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -3275,7 +3507,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C29" t="n">
         <v>12</v>
@@ -3286,7 +3518,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C30" t="n">
         <v>12</v>
@@ -3297,364 +3529,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" t="n">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C31"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
         <v>69</v>
-      </c>
-      <c r="C22" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>71</v>
-      </c>
-      <c r="C26" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C27" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>75</v>
       </c>
       <c r="C31" t="n">
         <v>12</v>

</xml_diff>